<commit_message>
updated benchmarker and presentation
</commit_message>
<xml_diff>
--- a/report/benchmark.xlsx
+++ b/report/benchmark.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="11475" windowHeight="6720"/>
+    <workbookView xWindow="240" yWindow="180" windowWidth="11475" windowHeight="6660"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="7">
   <si>
     <t>connected clients</t>
   </si>
@@ -252,11 +252,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="94073216"/>
-        <c:axId val="94074752"/>
+        <c:axId val="91417600"/>
+        <c:axId val="43385600"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="94073216"/>
+        <c:axId val="91417600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -266,7 +266,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="94074752"/>
+        <c:crossAx val="43385600"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -274,7 +274,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="94074752"/>
+        <c:axId val="43385600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -285,7 +285,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="94073216"/>
+        <c:crossAx val="91417600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -332,7 +332,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Blad1!$D$33</c:f>
+              <c:f>Blad1!$D$32</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -351,178 +351,178 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="58"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>200</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20</c:v>
+                  <c:v>300</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>30</c:v>
+                  <c:v>400</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>40</c:v>
+                  <c:v>500</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>50</c:v>
+                  <c:v>600</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>60</c:v>
+                  <c:v>700</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>70</c:v>
+                  <c:v>800</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>80</c:v>
+                  <c:v>900</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>90</c:v>
+                  <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>100</c:v>
+                  <c:v>1100</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>110</c:v>
+                  <c:v>1200</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>120</c:v>
+                  <c:v>1300</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>130</c:v>
+                  <c:v>1400</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>140</c:v>
+                  <c:v>1500</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>150</c:v>
+                  <c:v>1600</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>160</c:v>
+                  <c:v>1700</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>170</c:v>
+                  <c:v>1800</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>180</c:v>
+                  <c:v>1900</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>190</c:v>
+                  <c:v>2000</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>200</c:v>
+                  <c:v>2100</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>210</c:v>
+                  <c:v>2200</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>220</c:v>
+                  <c:v>2300</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>230</c:v>
+                  <c:v>2400</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>240</c:v>
+                  <c:v>2500</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>250</c:v>
+                  <c:v>2600</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>260</c:v>
+                  <c:v>2700</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>270</c:v>
+                  <c:v>2800</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>280</c:v>
+                  <c:v>2900</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>290</c:v>
+                  <c:v>3000</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>300</c:v>
+                  <c:v>3100</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>310</c:v>
+                  <c:v>3200</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>320</c:v>
+                  <c:v>3300</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>330</c:v>
+                  <c:v>3400</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>340</c:v>
+                  <c:v>3500</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>350</c:v>
+                  <c:v>3600</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>360</c:v>
+                  <c:v>3700</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>370</c:v>
+                  <c:v>3800</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>380</c:v>
+                  <c:v>3900</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>390</c:v>
+                  <c:v>4000</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>400</c:v>
+                  <c:v>4100</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>410</c:v>
+                  <c:v>4200</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>420</c:v>
+                  <c:v>4300</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>430</c:v>
+                  <c:v>4400</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>440</c:v>
+                  <c:v>4500</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>450</c:v>
+                  <c:v>4600</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>460</c:v>
+                  <c:v>4700</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>470</c:v>
+                  <c:v>4800</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>480</c:v>
+                  <c:v>4900</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>490</c:v>
+                  <c:v>5000</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>500</c:v>
+                  <c:v>5100</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>600</c:v>
+                  <c:v>5200</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>700</c:v>
+                  <c:v>5300</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>800</c:v>
+                  <c:v>5400</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>900</c:v>
+                  <c:v>5500</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>1000</c:v>
+                  <c:v>5600</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>1100</c:v>
+                  <c:v>5700</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>1200</c:v>
+                  <c:v>5800</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -543,16 +543,16 @@
                   <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>33</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>33</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>33</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>33</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>33</c:v>
@@ -561,7 +561,7 @@
                   <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>33</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>33</c:v>
@@ -582,130 +582,16 @@
                   <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>33</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="18">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="19">
                   <c:v>33</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>31</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>31</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>31</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>31</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>31</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>29</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>29</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>29</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>29</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>29</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>29</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>28</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>28</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>28</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>28</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>28</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>28</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>28</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>26</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>28</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>52</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>62</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>70</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>79</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>94</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -717,7 +603,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Blad1!$E$33</c:f>
+              <c:f>Blad1!$E$32</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -736,178 +622,178 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="58"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>200</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20</c:v>
+                  <c:v>300</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>30</c:v>
+                  <c:v>400</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>40</c:v>
+                  <c:v>500</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>50</c:v>
+                  <c:v>600</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>60</c:v>
+                  <c:v>700</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>70</c:v>
+                  <c:v>800</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>80</c:v>
+                  <c:v>900</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>90</c:v>
+                  <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>100</c:v>
+                  <c:v>1100</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>110</c:v>
+                  <c:v>1200</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>120</c:v>
+                  <c:v>1300</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>130</c:v>
+                  <c:v>1400</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>140</c:v>
+                  <c:v>1500</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>150</c:v>
+                  <c:v>1600</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>160</c:v>
+                  <c:v>1700</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>170</c:v>
+                  <c:v>1800</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>180</c:v>
+                  <c:v>1900</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>190</c:v>
+                  <c:v>2000</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>200</c:v>
+                  <c:v>2100</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>210</c:v>
+                  <c:v>2200</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>220</c:v>
+                  <c:v>2300</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>230</c:v>
+                  <c:v>2400</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>240</c:v>
+                  <c:v>2500</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>250</c:v>
+                  <c:v>2600</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>260</c:v>
+                  <c:v>2700</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>270</c:v>
+                  <c:v>2800</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>280</c:v>
+                  <c:v>2900</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>290</c:v>
+                  <c:v>3000</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>300</c:v>
+                  <c:v>3100</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>310</c:v>
+                  <c:v>3200</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>320</c:v>
+                  <c:v>3300</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>330</c:v>
+                  <c:v>3400</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>340</c:v>
+                  <c:v>3500</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>350</c:v>
+                  <c:v>3600</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>360</c:v>
+                  <c:v>3700</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>370</c:v>
+                  <c:v>3800</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>380</c:v>
+                  <c:v>3900</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>390</c:v>
+                  <c:v>4000</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>400</c:v>
+                  <c:v>4100</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>410</c:v>
+                  <c:v>4200</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>420</c:v>
+                  <c:v>4300</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>430</c:v>
+                  <c:v>4400</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>440</c:v>
+                  <c:v>4500</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>450</c:v>
+                  <c:v>4600</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>460</c:v>
+                  <c:v>4700</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>470</c:v>
+                  <c:v>4800</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>480</c:v>
+                  <c:v>4900</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>490</c:v>
+                  <c:v>5000</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>500</c:v>
+                  <c:v>5100</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>600</c:v>
+                  <c:v>5200</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>700</c:v>
+                  <c:v>5300</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>800</c:v>
+                  <c:v>5400</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>900</c:v>
+                  <c:v>5500</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>1000</c:v>
+                  <c:v>5600</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>1100</c:v>
+                  <c:v>5700</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>1200</c:v>
+                  <c:v>5800</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -919,16 +805,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="58"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>18</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>18</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>18</c:v>
@@ -937,160 +823,46 @@
                   <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>18</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>18</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>18</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>18</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>18</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>18</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>18</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>18</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>18</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>18</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>18</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>18</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>18</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>23</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>26</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>27</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>27</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>35</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>38</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>43</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>120</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1102,7 +874,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Blad1!$F$33</c:f>
+              <c:f>Blad1!$F$32</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1121,178 +893,178 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="58"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>200</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20</c:v>
+                  <c:v>300</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>30</c:v>
+                  <c:v>400</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>40</c:v>
+                  <c:v>500</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>50</c:v>
+                  <c:v>600</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>60</c:v>
+                  <c:v>700</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>70</c:v>
+                  <c:v>800</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>80</c:v>
+                  <c:v>900</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>90</c:v>
+                  <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>100</c:v>
+                  <c:v>1100</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>110</c:v>
+                  <c:v>1200</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>120</c:v>
+                  <c:v>1300</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>130</c:v>
+                  <c:v>1400</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>140</c:v>
+                  <c:v>1500</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>150</c:v>
+                  <c:v>1600</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>160</c:v>
+                  <c:v>1700</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>170</c:v>
+                  <c:v>1800</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>180</c:v>
+                  <c:v>1900</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>190</c:v>
+                  <c:v>2000</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>200</c:v>
+                  <c:v>2100</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>210</c:v>
+                  <c:v>2200</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>220</c:v>
+                  <c:v>2300</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>230</c:v>
+                  <c:v>2400</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>240</c:v>
+                  <c:v>2500</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>250</c:v>
+                  <c:v>2600</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>260</c:v>
+                  <c:v>2700</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>270</c:v>
+                  <c:v>2800</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>280</c:v>
+                  <c:v>2900</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>290</c:v>
+                  <c:v>3000</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>300</c:v>
+                  <c:v>3100</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>310</c:v>
+                  <c:v>3200</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>320</c:v>
+                  <c:v>3300</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>330</c:v>
+                  <c:v>3400</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>340</c:v>
+                  <c:v>3500</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>350</c:v>
+                  <c:v>3600</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>360</c:v>
+                  <c:v>3700</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>370</c:v>
+                  <c:v>3800</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>380</c:v>
+                  <c:v>3900</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>390</c:v>
+                  <c:v>4000</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>400</c:v>
+                  <c:v>4100</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>410</c:v>
+                  <c:v>4200</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>420</c:v>
+                  <c:v>4300</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>430</c:v>
+                  <c:v>4400</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>440</c:v>
+                  <c:v>4500</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>450</c:v>
+                  <c:v>4600</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>460</c:v>
+                  <c:v>4700</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>470</c:v>
+                  <c:v>4800</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>480</c:v>
+                  <c:v>4900</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>490</c:v>
+                  <c:v>5000</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>500</c:v>
+                  <c:v>5100</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>600</c:v>
+                  <c:v>5200</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>700</c:v>
+                  <c:v>5300</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>800</c:v>
+                  <c:v>5400</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>900</c:v>
+                  <c:v>5500</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>1000</c:v>
+                  <c:v>5600</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>1100</c:v>
+                  <c:v>5700</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>1200</c:v>
+                  <c:v>5800</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1303,180 +1075,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="58"/>
-                <c:pt idx="0">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>26</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>17</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1492,11 +1090,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="94100864"/>
-        <c:axId val="94102656"/>
+        <c:axId val="43432192"/>
+        <c:axId val="43433984"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="94100864"/>
+        <c:axId val="43432192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1506,7 +1104,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="94102656"/>
+        <c:crossAx val="43433984"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1514,7 +1112,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="94102656"/>
+        <c:axId val="43433984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1525,7 +1123,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="94100864"/>
+        <c:crossAx val="43432192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2768,11 +2366,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="95250688"/>
-        <c:axId val="95256576"/>
+        <c:axId val="43793024"/>
+        <c:axId val="43794816"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="95250688"/>
+        <c:axId val="43793024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2782,7 +2380,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95256576"/>
+        <c:crossAx val="43794816"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2790,7 +2388,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="95256576"/>
+        <c:axId val="43794816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2801,7 +2399,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95250688"/>
+        <c:crossAx val="43793024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3999,11 +3597,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="95294592"/>
-        <c:axId val="95296128"/>
+        <c:axId val="43820544"/>
+        <c:axId val="43822080"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="95294592"/>
+        <c:axId val="43820544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4013,7 +3611,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95296128"/>
+        <c:crossAx val="43822080"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4021,7 +3619,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="95296128"/>
+        <c:axId val="43822080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4032,7 +3630,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95294592"/>
+        <c:crossAx val="43820544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5203,11 +4801,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="95331840"/>
-        <c:axId val="95333376"/>
+        <c:axId val="45756800"/>
+        <c:axId val="45758336"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="95331840"/>
+        <c:axId val="45756800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5217,7 +4815,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95333376"/>
+        <c:crossAx val="45758336"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5225,7 +4823,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="95333376"/>
+        <c:axId val="45758336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5236,7 +4834,665 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95331840"/>
+        <c:crossAx val="45756800"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Blad1!$AF$37</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ping (ms)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Blad1!$AD$38:$AD$77</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="40"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1100</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1200</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1400</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1600</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1700</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1800</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1900</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2100</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2200</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2300</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2400</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2500</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2600</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2700</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2800</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2900</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>3100</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>3200</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>3300</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>3400</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>3500</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>3600</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>3700</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>3800</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>3900</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Blad1!$AF$38:$AF$77</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="40"/>
+                <c:pt idx="0">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>33</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Blad1!$AG$37</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>deviation (ms)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Blad1!$AG$38:$AG$77</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="40"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>17</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Blad1!$AH$37</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>FPS</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Blad1!$AH$38:$AH$77</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="40"/>
+                <c:pt idx="0">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>30</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="93623424"/>
+        <c:axId val="93624960"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="93623424"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="93624960"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="93624960"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="93623424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5293,15 +5549,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>476251</xdr:colOff>
-      <xdr:row>94</xdr:row>
-      <xdr:rowOff>188117</xdr:rowOff>
+      <xdr:colOff>77933</xdr:colOff>
+      <xdr:row>144</xdr:row>
+      <xdr:rowOff>66889</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>142875</xdr:colOff>
-      <xdr:row>120</xdr:row>
-      <xdr:rowOff>119062</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1788102</xdr:colOff>
+      <xdr:row>169</xdr:row>
+      <xdr:rowOff>188334</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5411,6 +5667,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>18338</xdr:colOff>
+      <xdr:row>78</xdr:row>
+      <xdr:rowOff>174300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>1277471</xdr:colOff>
+      <xdr:row>96</xdr:row>
+      <xdr:rowOff>159937</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Diagram 7"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -5706,10 +5992,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:Y93"/>
+  <dimension ref="B2:AH133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="W19" sqref="W19"/>
+    <sheetView tabSelected="1" topLeftCell="W58" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Z83" sqref="Z83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5734,6 +6020,11 @@
     <col min="23" max="23" width="25.5703125" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="7" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="6.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
@@ -5857,21 +6148,35 @@
         <v>240</v>
       </c>
     </row>
-    <row r="33" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B33" s="1" t="s">
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B32" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="C32" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D33" s="1" t="s">
+      <c r="D32" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E33" s="1" t="s">
+      <c r="E32" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F33" s="1" t="s">
+      <c r="F32" s="1" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B33">
+        <v>1</v>
+      </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
+      <c r="D33">
+        <v>33</v>
+      </c>
+      <c r="E33">
+        <v>1</v>
       </c>
       <c r="I33" s="1" t="s">
         <v>0</v>
@@ -5919,9 +6224,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B34">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="C34">
         <v>1</v>
@@ -5930,10 +6235,7 @@
         <v>33</v>
       </c>
       <c r="E34">
-        <v>2</v>
-      </c>
-      <c r="F34">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="I34">
         <v>1</v>
@@ -5981,9 +6283,9 @@
         <v>30</v>
       </c>
     </row>
-    <row r="35" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B35">
-        <v>10</v>
+        <v>200</v>
       </c>
       <c r="C35">
         <v>1</v>
@@ -5992,10 +6294,7 @@
         <v>33</v>
       </c>
       <c r="E35">
-        <v>18</v>
-      </c>
-      <c r="F35">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="I35">
         <v>10</v>
@@ -6043,9 +6342,9 @@
         <v>30</v>
       </c>
     </row>
-    <row r="36" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B36">
-        <v>20</v>
+        <v>300</v>
       </c>
       <c r="C36">
         <v>1</v>
@@ -6054,10 +6353,7 @@
         <v>33</v>
       </c>
       <c r="E36">
-        <v>18</v>
-      </c>
-      <c r="F36">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="I36">
         <v>20</v>
@@ -6105,21 +6401,18 @@
         <v>30</v>
       </c>
     </row>
-    <row r="37" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B37">
-        <v>30</v>
+        <v>400</v>
       </c>
       <c r="C37">
         <v>1</v>
       </c>
       <c r="D37">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E37">
-        <v>18</v>
-      </c>
-      <c r="F37">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="I37">
         <v>30</v>
@@ -6166,23 +6459,35 @@
       <c r="Y37">
         <v>30</v>
       </c>
-    </row>
-    <row r="38" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="AD37" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE37" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AF37" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AG37" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AH37" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B38">
-        <v>40</v>
+        <v>500</v>
       </c>
       <c r="C38">
         <v>1</v>
       </c>
       <c r="D38">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E38">
         <v>18</v>
       </c>
-      <c r="F38">
-        <v>30</v>
-      </c>
       <c r="I38">
         <v>40</v>
       </c>
@@ -6228,23 +6533,35 @@
       <c r="Y38">
         <v>30</v>
       </c>
-    </row>
-    <row r="39" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="AD38">
+        <v>1</v>
+      </c>
+      <c r="AE38">
+        <v>30</v>
+      </c>
+      <c r="AF38">
+        <v>33</v>
+      </c>
+      <c r="AG38">
+        <v>1</v>
+      </c>
+      <c r="AH38">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="39" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B39">
-        <v>50</v>
+        <v>600</v>
       </c>
       <c r="C39">
         <v>1</v>
       </c>
       <c r="D39">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E39">
         <v>18</v>
       </c>
-      <c r="F39">
-        <v>30</v>
-      </c>
       <c r="I39">
         <v>50</v>
       </c>
@@ -6290,22 +6607,34 @@
       <c r="Y39">
         <v>30</v>
       </c>
-    </row>
-    <row r="40" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="AD39">
+        <v>100</v>
+      </c>
+      <c r="AE39">
+        <v>30</v>
+      </c>
+      <c r="AF39">
+        <v>33</v>
+      </c>
+      <c r="AG39">
+        <v>1</v>
+      </c>
+      <c r="AH39">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="40" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B40">
-        <v>60</v>
+        <v>700</v>
       </c>
       <c r="C40">
         <v>1</v>
       </c>
       <c r="D40">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E40">
-        <v>18</v>
-      </c>
-      <c r="F40">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="I40">
         <v>60</v>
@@ -6352,10 +6681,25 @@
       <c r="Y40">
         <v>30</v>
       </c>
-    </row>
-    <row r="41" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="AD40">
+        <v>200</v>
+      </c>
+      <c r="AE40">
+        <v>30</v>
+      </c>
+      <c r="AF40">
+        <v>33</v>
+      </c>
+      <c r="AG40">
+        <v>1</v>
+      </c>
+      <c r="AH40">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="41" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B41">
-        <v>70</v>
+        <v>800</v>
       </c>
       <c r="C41">
         <v>1</v>
@@ -6364,10 +6708,7 @@
         <v>33</v>
       </c>
       <c r="E41">
-        <v>18</v>
-      </c>
-      <c r="F41">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="I41">
         <v>70</v>
@@ -6414,10 +6755,25 @@
       <c r="Y41">
         <v>30</v>
       </c>
-    </row>
-    <row r="42" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="AD41">
+        <v>300</v>
+      </c>
+      <c r="AE41">
+        <v>30</v>
+      </c>
+      <c r="AF41">
+        <v>33</v>
+      </c>
+      <c r="AG41">
+        <v>17</v>
+      </c>
+      <c r="AH41">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="42" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B42">
-        <v>80</v>
+        <v>900</v>
       </c>
       <c r="C42">
         <v>1</v>
@@ -6426,10 +6782,7 @@
         <v>33</v>
       </c>
       <c r="E42">
-        <v>18</v>
-      </c>
-      <c r="F42">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="I42">
         <v>80</v>
@@ -6476,22 +6829,34 @@
       <c r="Y42">
         <v>30</v>
       </c>
-    </row>
-    <row r="43" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="AD42">
+        <v>400</v>
+      </c>
+      <c r="AE42">
+        <v>30</v>
+      </c>
+      <c r="AF42">
+        <v>35</v>
+      </c>
+      <c r="AG42">
+        <v>17</v>
+      </c>
+      <c r="AH42">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="43" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B43">
-        <v>90</v>
+        <v>1000</v>
       </c>
       <c r="C43">
         <v>1</v>
       </c>
       <c r="D43">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E43">
-        <v>18</v>
-      </c>
-      <c r="F43">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="I43">
         <v>90</v>
@@ -6538,10 +6903,25 @@
       <c r="Y43">
         <v>30</v>
       </c>
-    </row>
-    <row r="44" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="AD43">
+        <v>500</v>
+      </c>
+      <c r="AE43">
+        <v>30</v>
+      </c>
+      <c r="AF43">
+        <v>35</v>
+      </c>
+      <c r="AG43">
+        <v>18</v>
+      </c>
+      <c r="AH43">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="44" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B44">
-        <v>100</v>
+        <v>1100</v>
       </c>
       <c r="C44">
         <v>1</v>
@@ -6550,10 +6930,7 @@
         <v>33</v>
       </c>
       <c r="E44">
-        <v>18</v>
-      </c>
-      <c r="F44">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="I44">
         <v>100</v>
@@ -6600,10 +6977,25 @@
       <c r="Y44">
         <v>30</v>
       </c>
-    </row>
-    <row r="45" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="AD44">
+        <v>600</v>
+      </c>
+      <c r="AE44">
+        <v>30</v>
+      </c>
+      <c r="AF44">
+        <v>35</v>
+      </c>
+      <c r="AG44">
+        <v>18</v>
+      </c>
+      <c r="AH44">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="45" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B45">
-        <v>110</v>
+        <v>1200</v>
       </c>
       <c r="C45">
         <v>1</v>
@@ -6612,10 +7004,7 @@
         <v>33</v>
       </c>
       <c r="E45">
-        <v>18</v>
-      </c>
-      <c r="F45">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="I45">
         <v>110</v>
@@ -6662,10 +7051,25 @@
       <c r="Y45">
         <v>30</v>
       </c>
-    </row>
-    <row r="46" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="AD45">
+        <v>700</v>
+      </c>
+      <c r="AE45">
+        <v>30</v>
+      </c>
+      <c r="AF45">
+        <v>34</v>
+      </c>
+      <c r="AG45">
+        <v>17</v>
+      </c>
+      <c r="AH45">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="46" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B46">
-        <v>120</v>
+        <v>1300</v>
       </c>
       <c r="C46">
         <v>1</v>
@@ -6674,10 +7078,7 @@
         <v>33</v>
       </c>
       <c r="E46">
-        <v>18</v>
-      </c>
-      <c r="F46">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="I46">
         <v>120</v>
@@ -6724,10 +7125,25 @@
       <c r="Y46">
         <v>30</v>
       </c>
-    </row>
-    <row r="47" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="AD46">
+        <v>800</v>
+      </c>
+      <c r="AE46">
+        <v>30</v>
+      </c>
+      <c r="AF46">
+        <v>33</v>
+      </c>
+      <c r="AG46">
+        <v>16</v>
+      </c>
+      <c r="AH46">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="47" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B47">
-        <v>130</v>
+        <v>1400</v>
       </c>
       <c r="C47">
         <v>1</v>
@@ -6736,10 +7152,7 @@
         <v>33</v>
       </c>
       <c r="E47">
-        <v>18</v>
-      </c>
-      <c r="F47">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="I47">
         <v>130</v>
@@ -6786,10 +7199,25 @@
       <c r="Y47">
         <v>30</v>
       </c>
-    </row>
-    <row r="48" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="AD47">
+        <v>900</v>
+      </c>
+      <c r="AE47">
+        <v>30</v>
+      </c>
+      <c r="AF47">
+        <v>33</v>
+      </c>
+      <c r="AG47">
+        <v>15</v>
+      </c>
+      <c r="AH47">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="48" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B48">
-        <v>140</v>
+        <v>1500</v>
       </c>
       <c r="C48">
         <v>1</v>
@@ -6798,10 +7226,7 @@
         <v>33</v>
       </c>
       <c r="E48">
-        <v>18</v>
-      </c>
-      <c r="F48">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="I48">
         <v>140</v>
@@ -6848,10 +7273,25 @@
       <c r="Y48">
         <v>30</v>
       </c>
-    </row>
-    <row r="49" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="AD48">
+        <v>1000</v>
+      </c>
+      <c r="AE48">
+        <v>30</v>
+      </c>
+      <c r="AF48">
+        <v>34</v>
+      </c>
+      <c r="AG48">
+        <v>17</v>
+      </c>
+      <c r="AH48">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="49" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B49">
-        <v>150</v>
+        <v>1600</v>
       </c>
       <c r="C49">
         <v>1</v>
@@ -6860,10 +7300,7 @@
         <v>33</v>
       </c>
       <c r="E49">
-        <v>18</v>
-      </c>
-      <c r="F49">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="I49">
         <v>150</v>
@@ -6910,22 +7347,34 @@
       <c r="Y49">
         <v>30</v>
       </c>
-    </row>
-    <row r="50" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="AD49">
+        <v>1100</v>
+      </c>
+      <c r="AE49">
+        <v>30</v>
+      </c>
+      <c r="AF49">
+        <v>33</v>
+      </c>
+      <c r="AG49">
+        <v>16</v>
+      </c>
+      <c r="AH49">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="50" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B50">
-        <v>160</v>
+        <v>1700</v>
       </c>
       <c r="C50">
         <v>1</v>
       </c>
       <c r="D50">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E50">
-        <v>18</v>
-      </c>
-      <c r="F50">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="I50">
         <v>160</v>
@@ -6972,10 +7421,25 @@
       <c r="Y50">
         <v>30</v>
       </c>
-    </row>
-    <row r="51" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="AD50">
+        <v>1200</v>
+      </c>
+      <c r="AE50">
+        <v>30</v>
+      </c>
+      <c r="AF50">
+        <v>33</v>
+      </c>
+      <c r="AG50">
+        <v>16</v>
+      </c>
+      <c r="AH50">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="51" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B51">
-        <v>170</v>
+        <v>1800</v>
       </c>
       <c r="C51">
         <v>1</v>
@@ -6984,10 +7448,7 @@
         <v>33</v>
       </c>
       <c r="E51">
-        <v>18</v>
-      </c>
-      <c r="F51">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="I51">
         <v>170</v>
@@ -7034,22 +7495,34 @@
       <c r="Y51">
         <v>30</v>
       </c>
-    </row>
-    <row r="52" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="AD51">
+        <v>1300</v>
+      </c>
+      <c r="AE51">
+        <v>30</v>
+      </c>
+      <c r="AF51">
+        <v>33</v>
+      </c>
+      <c r="AG51">
+        <v>16</v>
+      </c>
+      <c r="AH51">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="52" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B52">
-        <v>180</v>
+        <v>1900</v>
       </c>
       <c r="C52">
         <v>1</v>
       </c>
       <c r="D52">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E52">
-        <v>18</v>
-      </c>
-      <c r="F52">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="I52">
         <v>180</v>
@@ -7096,22 +7569,34 @@
       <c r="Y52">
         <v>30</v>
       </c>
-    </row>
-    <row r="53" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="AD52">
+        <v>1400</v>
+      </c>
+      <c r="AE52">
+        <v>30</v>
+      </c>
+      <c r="AF52">
+        <v>33</v>
+      </c>
+      <c r="AG52">
+        <v>17</v>
+      </c>
+      <c r="AH52">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="53" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B53">
-        <v>190</v>
+        <v>2000</v>
       </c>
       <c r="C53">
         <v>1</v>
       </c>
       <c r="D53">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E53">
-        <v>18</v>
-      </c>
-      <c r="F53">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="I53">
         <v>190</v>
@@ -7158,22 +7643,28 @@
       <c r="Y53">
         <v>30</v>
       </c>
-    </row>
-    <row r="54" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="AD53">
+        <v>1500</v>
+      </c>
+      <c r="AE53">
+        <v>30</v>
+      </c>
+      <c r="AF53">
+        <v>33</v>
+      </c>
+      <c r="AG53">
+        <v>16</v>
+      </c>
+      <c r="AH53">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="54" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B54">
-        <v>200</v>
+        <v>2100</v>
       </c>
       <c r="C54">
         <v>1</v>
-      </c>
-      <c r="D54">
-        <v>32</v>
-      </c>
-      <c r="E54">
-        <v>18</v>
-      </c>
-      <c r="F54">
-        <v>30</v>
       </c>
       <c r="I54">
         <v>200</v>
@@ -7220,22 +7711,28 @@
       <c r="Y54">
         <v>28</v>
       </c>
-    </row>
-    <row r="55" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="AD54">
+        <v>1600</v>
+      </c>
+      <c r="AE54">
+        <v>30</v>
+      </c>
+      <c r="AF54">
+        <v>33</v>
+      </c>
+      <c r="AG54">
+        <v>15</v>
+      </c>
+      <c r="AH54">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="55" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B55">
-        <v>210</v>
+        <v>2200</v>
       </c>
       <c r="C55">
         <v>1</v>
-      </c>
-      <c r="D55">
-        <v>32</v>
-      </c>
-      <c r="E55">
-        <v>18</v>
-      </c>
-      <c r="F55">
-        <v>30</v>
       </c>
       <c r="I55">
         <v>210</v>
@@ -7282,22 +7779,28 @@
       <c r="Y55">
         <v>26</v>
       </c>
-    </row>
-    <row r="56" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="AD55">
+        <v>1700</v>
+      </c>
+      <c r="AE55">
+        <v>30</v>
+      </c>
+      <c r="AF55">
+        <v>34</v>
+      </c>
+      <c r="AG55">
+        <v>16</v>
+      </c>
+      <c r="AH55">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="56" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B56">
-        <v>220</v>
+        <v>2300</v>
       </c>
       <c r="C56">
         <v>1</v>
-      </c>
-      <c r="D56">
-        <v>32</v>
-      </c>
-      <c r="E56">
-        <v>18</v>
-      </c>
-      <c r="F56">
-        <v>30</v>
       </c>
       <c r="I56">
         <v>220</v>
@@ -7344,22 +7847,28 @@
       <c r="Y56">
         <v>24</v>
       </c>
-    </row>
-    <row r="57" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="AD56">
+        <v>1800</v>
+      </c>
+      <c r="AE56">
+        <v>30</v>
+      </c>
+      <c r="AF56">
+        <v>33</v>
+      </c>
+      <c r="AG56">
+        <v>17</v>
+      </c>
+      <c r="AH56">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="57" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B57">
-        <v>230</v>
+        <v>2400</v>
       </c>
       <c r="C57">
         <v>1</v>
-      </c>
-      <c r="D57">
-        <v>32</v>
-      </c>
-      <c r="E57">
-        <v>18</v>
-      </c>
-      <c r="F57">
-        <v>30</v>
       </c>
       <c r="I57">
         <v>230</v>
@@ -7406,22 +7915,28 @@
       <c r="Y57">
         <v>24</v>
       </c>
-    </row>
-    <row r="58" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="AD57">
+        <v>1900</v>
+      </c>
+      <c r="AE57">
+        <v>30</v>
+      </c>
+      <c r="AF57">
+        <v>34</v>
+      </c>
+      <c r="AG57">
+        <v>16</v>
+      </c>
+      <c r="AH57">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="58" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B58">
-        <v>240</v>
+        <v>2500</v>
       </c>
       <c r="C58">
         <v>1</v>
-      </c>
-      <c r="D58">
-        <v>32</v>
-      </c>
-      <c r="E58">
-        <v>18</v>
-      </c>
-      <c r="F58">
-        <v>30</v>
       </c>
       <c r="I58">
         <v>240</v>
@@ -7468,22 +7983,28 @@
       <c r="Y58">
         <v>23</v>
       </c>
-    </row>
-    <row r="59" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="AD58">
+        <v>2000</v>
+      </c>
+      <c r="AE58">
+        <v>30</v>
+      </c>
+      <c r="AF58">
+        <v>33</v>
+      </c>
+      <c r="AG58">
+        <v>17</v>
+      </c>
+      <c r="AH58">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="59" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B59">
-        <v>250</v>
+        <v>2600</v>
       </c>
       <c r="C59">
         <v>1</v>
-      </c>
-      <c r="D59">
-        <v>31</v>
-      </c>
-      <c r="E59">
-        <v>18</v>
-      </c>
-      <c r="F59">
-        <v>30</v>
       </c>
       <c r="I59">
         <v>250</v>
@@ -7530,22 +8051,28 @@
       <c r="Y59">
         <v>23</v>
       </c>
-    </row>
-    <row r="60" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="AD59">
+        <v>2100</v>
+      </c>
+      <c r="AE59">
+        <v>30</v>
+      </c>
+      <c r="AF59">
+        <v>33</v>
+      </c>
+      <c r="AG59">
+        <v>16</v>
+      </c>
+      <c r="AH59">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="60" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B60">
-        <v>260</v>
+        <v>2700</v>
       </c>
       <c r="C60">
         <v>1</v>
-      </c>
-      <c r="D60">
-        <v>31</v>
-      </c>
-      <c r="E60">
-        <v>18</v>
-      </c>
-      <c r="F60">
-        <v>30</v>
       </c>
       <c r="I60">
         <v>260</v>
@@ -7592,22 +8119,28 @@
       <c r="Y60">
         <v>23</v>
       </c>
-    </row>
-    <row r="61" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="AD60">
+        <v>2200</v>
+      </c>
+      <c r="AE60">
+        <v>30</v>
+      </c>
+      <c r="AF60">
+        <v>33</v>
+      </c>
+      <c r="AG60">
+        <v>17</v>
+      </c>
+      <c r="AH60">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="61" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B61">
-        <v>270</v>
+        <v>2800</v>
       </c>
       <c r="C61">
         <v>1</v>
-      </c>
-      <c r="D61">
-        <v>31</v>
-      </c>
-      <c r="E61">
-        <v>18</v>
-      </c>
-      <c r="F61">
-        <v>30</v>
       </c>
       <c r="I61">
         <v>270</v>
@@ -7654,22 +8187,28 @@
       <c r="Y61">
         <v>23</v>
       </c>
-    </row>
-    <row r="62" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="AD61">
+        <v>2300</v>
+      </c>
+      <c r="AE61">
+        <v>30</v>
+      </c>
+      <c r="AF61">
+        <v>34</v>
+      </c>
+      <c r="AG61">
+        <v>16</v>
+      </c>
+      <c r="AH61">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="62" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B62">
-        <v>280</v>
+        <v>2900</v>
       </c>
       <c r="C62">
         <v>1</v>
-      </c>
-      <c r="D62">
-        <v>31</v>
-      </c>
-      <c r="E62">
-        <v>18</v>
-      </c>
-      <c r="F62">
-        <v>30</v>
       </c>
       <c r="I62">
         <v>280</v>
@@ -7716,22 +8255,28 @@
       <c r="Y62">
         <v>23</v>
       </c>
-    </row>
-    <row r="63" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="AD62">
+        <v>2400</v>
+      </c>
+      <c r="AE62">
+        <v>30</v>
+      </c>
+      <c r="AF62">
+        <v>34</v>
+      </c>
+      <c r="AG62">
+        <v>16</v>
+      </c>
+      <c r="AH62">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="63" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B63">
-        <v>290</v>
+        <v>3000</v>
       </c>
       <c r="C63">
         <v>1</v>
-      </c>
-      <c r="D63">
-        <v>31</v>
-      </c>
-      <c r="E63">
-        <v>18</v>
-      </c>
-      <c r="F63">
-        <v>30</v>
       </c>
       <c r="I63">
         <v>290</v>
@@ -7778,22 +8323,28 @@
       <c r="Y63">
         <v>24</v>
       </c>
-    </row>
-    <row r="64" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="AD63">
+        <v>2500</v>
+      </c>
+      <c r="AE63">
+        <v>30</v>
+      </c>
+      <c r="AF63">
+        <v>34</v>
+      </c>
+      <c r="AG63">
+        <v>16</v>
+      </c>
+      <c r="AH63">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="64" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B64">
-        <v>300</v>
+        <v>3100</v>
       </c>
       <c r="C64">
         <v>1</v>
-      </c>
-      <c r="D64">
-        <v>30</v>
-      </c>
-      <c r="E64">
-        <v>18</v>
-      </c>
-      <c r="F64">
-        <v>30</v>
       </c>
       <c r="I64">
         <v>300</v>
@@ -7840,22 +8391,28 @@
       <c r="Y64">
         <v>25</v>
       </c>
-    </row>
-    <row r="65" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="AD64">
+        <v>2600</v>
+      </c>
+      <c r="AE64">
+        <v>30</v>
+      </c>
+      <c r="AF64">
+        <v>33</v>
+      </c>
+      <c r="AG64">
+        <v>17</v>
+      </c>
+      <c r="AH64">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="65" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B65">
-        <v>310</v>
+        <v>3200</v>
       </c>
       <c r="C65">
         <v>1</v>
-      </c>
-      <c r="D65">
-        <v>30</v>
-      </c>
-      <c r="E65">
-        <v>18</v>
-      </c>
-      <c r="F65">
-        <v>30</v>
       </c>
       <c r="I65">
         <v>310</v>
@@ -7902,22 +8459,28 @@
       <c r="Y65">
         <v>25</v>
       </c>
-    </row>
-    <row r="66" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="AD65">
+        <v>2700</v>
+      </c>
+      <c r="AE65">
+        <v>30</v>
+      </c>
+      <c r="AF65">
+        <v>33</v>
+      </c>
+      <c r="AG65">
+        <v>16</v>
+      </c>
+      <c r="AH65">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="66" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B66">
-        <v>320</v>
+        <v>3300</v>
       </c>
       <c r="C66">
         <v>1</v>
-      </c>
-      <c r="D66">
-        <v>30</v>
-      </c>
-      <c r="E66">
-        <v>18</v>
-      </c>
-      <c r="F66">
-        <v>30</v>
       </c>
       <c r="I66">
         <v>320</v>
@@ -7964,22 +8527,28 @@
       <c r="Y66">
         <v>25</v>
       </c>
-    </row>
-    <row r="67" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="AD66">
+        <v>2800</v>
+      </c>
+      <c r="AE66">
+        <v>30</v>
+      </c>
+      <c r="AF66">
+        <v>33</v>
+      </c>
+      <c r="AG66">
+        <v>17</v>
+      </c>
+      <c r="AH66">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="67" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B67">
-        <v>330</v>
+        <v>3400</v>
       </c>
       <c r="C67">
         <v>1</v>
-      </c>
-      <c r="D67">
-        <v>30</v>
-      </c>
-      <c r="E67">
-        <v>18</v>
-      </c>
-      <c r="F67">
-        <v>30</v>
       </c>
       <c r="I67">
         <v>330</v>
@@ -8026,22 +8595,28 @@
       <c r="Y67">
         <v>24</v>
       </c>
-    </row>
-    <row r="68" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="AD67">
+        <v>2900</v>
+      </c>
+      <c r="AE67">
+        <v>30</v>
+      </c>
+      <c r="AF67">
+        <v>33</v>
+      </c>
+      <c r="AG67">
+        <v>17</v>
+      </c>
+      <c r="AH67">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="68" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B68">
-        <v>340</v>
+        <v>3500</v>
       </c>
       <c r="C68">
         <v>1</v>
-      </c>
-      <c r="D68">
-        <v>30</v>
-      </c>
-      <c r="E68">
-        <v>18</v>
-      </c>
-      <c r="F68">
-        <v>30</v>
       </c>
       <c r="I68">
         <v>340</v>
@@ -8088,22 +8663,28 @@
       <c r="Y68">
         <v>23</v>
       </c>
-    </row>
-    <row r="69" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="AD68">
+        <v>3000</v>
+      </c>
+      <c r="AE68">
+        <v>30</v>
+      </c>
+      <c r="AF68">
+        <v>34</v>
+      </c>
+      <c r="AG68">
+        <v>17</v>
+      </c>
+      <c r="AH68">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="69" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B69">
-        <v>350</v>
+        <v>3600</v>
       </c>
       <c r="C69">
         <v>1</v>
-      </c>
-      <c r="D69">
-        <v>30</v>
-      </c>
-      <c r="E69">
-        <v>19</v>
-      </c>
-      <c r="F69">
-        <v>30</v>
       </c>
       <c r="I69">
         <v>350</v>
@@ -8150,22 +8731,28 @@
       <c r="Y69">
         <v>23</v>
       </c>
-    </row>
-    <row r="70" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="AD69">
+        <v>3100</v>
+      </c>
+      <c r="AE69">
+        <v>30</v>
+      </c>
+      <c r="AF69">
+        <v>34</v>
+      </c>
+      <c r="AG69">
+        <v>16</v>
+      </c>
+      <c r="AH69">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="70" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B70">
-        <v>360</v>
+        <v>3700</v>
       </c>
       <c r="C70">
         <v>1</v>
-      </c>
-      <c r="D70">
-        <v>30</v>
-      </c>
-      <c r="E70">
-        <v>20</v>
-      </c>
-      <c r="F70">
-        <v>30</v>
       </c>
       <c r="I70">
         <v>360</v>
@@ -8212,22 +8799,28 @@
       <c r="Y70">
         <v>22</v>
       </c>
-    </row>
-    <row r="71" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="AD70">
+        <v>3200</v>
+      </c>
+      <c r="AE70">
+        <v>30</v>
+      </c>
+      <c r="AF70">
+        <v>33</v>
+      </c>
+      <c r="AG70">
+        <v>16</v>
+      </c>
+      <c r="AH70">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="71" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B71">
-        <v>370</v>
+        <v>3800</v>
       </c>
       <c r="C71">
         <v>1</v>
-      </c>
-      <c r="D71">
-        <v>30</v>
-      </c>
-      <c r="E71">
-        <v>22</v>
-      </c>
-      <c r="F71">
-        <v>30</v>
       </c>
       <c r="I71">
         <v>370</v>
@@ -8274,22 +8867,28 @@
       <c r="Y71">
         <v>21</v>
       </c>
-    </row>
-    <row r="72" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="AD71">
+        <v>3300</v>
+      </c>
+      <c r="AE71">
+        <v>30</v>
+      </c>
+      <c r="AF71">
+        <v>33</v>
+      </c>
+      <c r="AG71">
+        <v>16</v>
+      </c>
+      <c r="AH71">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="72" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B72">
-        <v>380</v>
+        <v>3900</v>
       </c>
       <c r="C72">
         <v>1</v>
-      </c>
-      <c r="D72">
-        <v>29</v>
-      </c>
-      <c r="E72">
-        <v>22</v>
-      </c>
-      <c r="F72">
-        <v>30</v>
       </c>
       <c r="I72">
         <v>380</v>
@@ -8336,22 +8935,28 @@
       <c r="Y72">
         <v>21</v>
       </c>
-    </row>
-    <row r="73" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="AD72">
+        <v>3400</v>
+      </c>
+      <c r="AE72">
+        <v>30</v>
+      </c>
+      <c r="AF72">
+        <v>34</v>
+      </c>
+      <c r="AG72">
+        <v>16</v>
+      </c>
+      <c r="AH72">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="73" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B73">
-        <v>390</v>
+        <v>4000</v>
       </c>
       <c r="C73">
         <v>1</v>
-      </c>
-      <c r="D73">
-        <v>29</v>
-      </c>
-      <c r="E73">
-        <v>23</v>
-      </c>
-      <c r="F73">
-        <v>30</v>
       </c>
       <c r="I73">
         <v>390</v>
@@ -8398,22 +9003,28 @@
       <c r="Y73">
         <v>18</v>
       </c>
-    </row>
-    <row r="74" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="AD73">
+        <v>3500</v>
+      </c>
+      <c r="AE73">
+        <v>30</v>
+      </c>
+      <c r="AF73">
+        <v>33</v>
+      </c>
+      <c r="AG73">
+        <v>17</v>
+      </c>
+      <c r="AH73">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="74" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B74">
-        <v>400</v>
+        <v>4100</v>
       </c>
       <c r="C74">
         <v>1</v>
-      </c>
-      <c r="D74">
-        <v>29</v>
-      </c>
-      <c r="E74">
-        <v>24</v>
-      </c>
-      <c r="F74">
-        <v>30</v>
       </c>
       <c r="I74">
         <v>400</v>
@@ -8460,22 +9071,28 @@
       <c r="Y74">
         <v>15</v>
       </c>
-    </row>
-    <row r="75" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="AD74">
+        <v>3600</v>
+      </c>
+      <c r="AE74">
+        <v>30</v>
+      </c>
+      <c r="AF74">
+        <v>34</v>
+      </c>
+      <c r="AG74">
+        <v>17</v>
+      </c>
+      <c r="AH74">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="75" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B75">
-        <v>410</v>
+        <v>4200</v>
       </c>
       <c r="C75">
         <v>1</v>
-      </c>
-      <c r="D75">
-        <v>29</v>
-      </c>
-      <c r="E75">
-        <v>24</v>
-      </c>
-      <c r="F75">
-        <v>30</v>
       </c>
       <c r="I75">
         <v>410</v>
@@ -8522,22 +9139,28 @@
       <c r="Y75">
         <v>15</v>
       </c>
-    </row>
-    <row r="76" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="AD75">
+        <v>3700</v>
+      </c>
+      <c r="AE75">
+        <v>30</v>
+      </c>
+      <c r="AF75">
+        <v>34</v>
+      </c>
+      <c r="AG75">
+        <v>16</v>
+      </c>
+      <c r="AH75">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="76" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B76">
-        <v>420</v>
+        <v>4300</v>
       </c>
       <c r="C76">
         <v>1</v>
-      </c>
-      <c r="D76">
-        <v>29</v>
-      </c>
-      <c r="E76">
-        <v>24</v>
-      </c>
-      <c r="F76">
-        <v>30</v>
       </c>
       <c r="I76">
         <v>420</v>
@@ -8584,22 +9207,28 @@
       <c r="Y76">
         <v>15</v>
       </c>
-    </row>
-    <row r="77" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="AD76">
+        <v>3800</v>
+      </c>
+      <c r="AE76">
+        <v>30</v>
+      </c>
+      <c r="AF76">
+        <v>33</v>
+      </c>
+      <c r="AG76">
+        <v>16</v>
+      </c>
+      <c r="AH76">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="77" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B77">
-        <v>430</v>
+        <v>4400</v>
       </c>
       <c r="C77">
         <v>1</v>
-      </c>
-      <c r="D77">
-        <v>29</v>
-      </c>
-      <c r="E77">
-        <v>24</v>
-      </c>
-      <c r="F77">
-        <v>30</v>
       </c>
       <c r="I77">
         <v>430</v>
@@ -8646,22 +9275,28 @@
       <c r="Y77">
         <v>15</v>
       </c>
-    </row>
-    <row r="78" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="AD77">
+        <v>3900</v>
+      </c>
+      <c r="AE77">
+        <v>30</v>
+      </c>
+      <c r="AF77">
+        <v>33</v>
+      </c>
+      <c r="AG77">
+        <v>17</v>
+      </c>
+      <c r="AH77">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="78" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B78">
-        <v>440</v>
+        <v>4500</v>
       </c>
       <c r="C78">
         <v>1</v>
-      </c>
-      <c r="D78">
-        <v>28</v>
-      </c>
-      <c r="E78">
-        <v>25</v>
-      </c>
-      <c r="F78">
-        <v>30</v>
       </c>
       <c r="I78">
         <v>440</v>
@@ -8709,21 +9344,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="79" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B79">
-        <v>450</v>
+        <v>4600</v>
       </c>
       <c r="C79">
         <v>1</v>
-      </c>
-      <c r="D79">
-        <v>28</v>
-      </c>
-      <c r="E79">
-        <v>25</v>
-      </c>
-      <c r="F79">
-        <v>30</v>
       </c>
       <c r="I79">
         <v>450</v>
@@ -8771,21 +9397,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="80" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B80">
-        <v>460</v>
+        <v>4700</v>
       </c>
       <c r="C80">
         <v>1</v>
-      </c>
-      <c r="D80">
-        <v>28</v>
-      </c>
-      <c r="E80">
-        <v>25</v>
-      </c>
-      <c r="F80">
-        <v>30</v>
       </c>
       <c r="I80">
         <v>460</v>
@@ -8835,19 +9452,10 @@
     </row>
     <row r="81" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B81">
-        <v>470</v>
+        <v>4800</v>
       </c>
       <c r="C81">
         <v>1</v>
-      </c>
-      <c r="D81">
-        <v>28</v>
-      </c>
-      <c r="E81">
-        <v>25</v>
-      </c>
-      <c r="F81">
-        <v>30</v>
       </c>
       <c r="I81">
         <v>470</v>
@@ -8897,19 +9505,10 @@
     </row>
     <row r="82" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B82">
-        <v>480</v>
+        <v>4900</v>
       </c>
       <c r="C82">
         <v>1</v>
-      </c>
-      <c r="D82">
-        <v>28</v>
-      </c>
-      <c r="E82">
-        <v>26</v>
-      </c>
-      <c r="F82">
-        <v>30</v>
       </c>
       <c r="I82">
         <v>480</v>
@@ -8959,19 +9558,10 @@
     </row>
     <row r="83" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B83">
-        <v>490</v>
+        <v>5000</v>
       </c>
       <c r="C83">
         <v>1</v>
-      </c>
-      <c r="D83">
-        <v>28</v>
-      </c>
-      <c r="E83">
-        <v>27</v>
-      </c>
-      <c r="F83">
-        <v>30</v>
       </c>
       <c r="I83">
         <v>490</v>
@@ -9021,19 +9611,10 @@
     </row>
     <row r="84" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B84">
-        <v>500</v>
+        <v>5100</v>
       </c>
       <c r="C84">
         <v>1</v>
-      </c>
-      <c r="D84">
-        <v>28</v>
-      </c>
-      <c r="E84">
-        <v>27</v>
-      </c>
-      <c r="F84">
-        <v>30</v>
       </c>
       <c r="I84">
         <v>500</v>
@@ -9083,19 +9664,10 @@
     </row>
     <row r="85" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B85">
-        <v>600</v>
+        <v>5200</v>
       </c>
       <c r="C85">
         <v>1</v>
-      </c>
-      <c r="D85">
-        <v>26</v>
-      </c>
-      <c r="E85">
-        <v>30</v>
-      </c>
-      <c r="F85">
-        <v>30</v>
       </c>
       <c r="I85">
         <v>600</v>
@@ -9145,19 +9717,10 @@
     </row>
     <row r="86" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B86">
-        <v>700</v>
+        <v>5300</v>
       </c>
       <c r="C86">
         <v>1</v>
-      </c>
-      <c r="D86">
-        <v>28</v>
-      </c>
-      <c r="E86">
-        <v>32</v>
-      </c>
-      <c r="F86">
-        <v>30</v>
       </c>
       <c r="I86">
         <v>700</v>
@@ -9201,19 +9764,10 @@
     </row>
     <row r="87" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B87">
-        <v>800</v>
+        <v>5400</v>
       </c>
       <c r="C87">
         <v>1</v>
-      </c>
-      <c r="D87">
-        <v>52</v>
-      </c>
-      <c r="E87">
-        <v>35</v>
-      </c>
-      <c r="F87">
-        <v>30</v>
       </c>
       <c r="I87">
         <v>800</v>
@@ -9254,19 +9808,10 @@
     </row>
     <row r="88" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B88">
-        <v>900</v>
+        <v>5500</v>
       </c>
       <c r="C88">
         <v>1</v>
-      </c>
-      <c r="D88">
-        <v>62</v>
-      </c>
-      <c r="E88">
-        <v>38</v>
-      </c>
-      <c r="F88">
-        <v>30</v>
       </c>
       <c r="I88">
         <v>900</v>
@@ -9307,19 +9852,10 @@
     </row>
     <row r="89" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B89">
-        <v>1000</v>
+        <v>5600</v>
       </c>
       <c r="C89">
         <v>1</v>
-      </c>
-      <c r="D89">
-        <v>70</v>
-      </c>
-      <c r="E89">
-        <v>43</v>
-      </c>
-      <c r="F89">
-        <v>26</v>
       </c>
       <c r="I89">
         <v>1000</v>
@@ -9357,19 +9893,10 @@
     </row>
     <row r="90" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B90">
-        <v>1100</v>
+        <v>5700</v>
       </c>
       <c r="C90">
         <v>1</v>
-      </c>
-      <c r="D90">
-        <v>79</v>
-      </c>
-      <c r="E90">
-        <v>80</v>
-      </c>
-      <c r="F90">
-        <v>20</v>
       </c>
       <c r="I90">
         <v>1100</v>
@@ -9401,19 +9928,10 @@
     </row>
     <row r="91" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B91">
-        <v>1200</v>
+        <v>5800</v>
       </c>
       <c r="C91">
         <v>1</v>
-      </c>
-      <c r="D91">
-        <v>94</v>
-      </c>
-      <c r="E91">
-        <v>120</v>
-      </c>
-      <c r="F91">
-        <v>17</v>
       </c>
       <c r="I91">
         <v>1200</v>
@@ -9444,8 +9962,12 @@
       </c>
     </row>
     <row r="92" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B92" s="2"/>
-      <c r="C92" s="2"/>
+      <c r="B92">
+        <v>5900</v>
+      </c>
+      <c r="C92">
+        <v>1</v>
+      </c>
       <c r="D92" s="2"/>
       <c r="E92" s="2"/>
       <c r="F92" s="2"/>
@@ -9484,6 +10006,12 @@
       <c r="Y92" s="2"/>
     </row>
     <row r="93" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B93">
+        <v>6000</v>
+      </c>
+      <c r="C93">
+        <v>1</v>
+      </c>
       <c r="I93">
         <v>1400</v>
       </c>
@@ -9510,6 +10038,326 @@
       </c>
       <c r="V93">
         <v>30</v>
+      </c>
+    </row>
+    <row r="94" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B94">
+        <v>6100</v>
+      </c>
+      <c r="C94">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B95">
+        <v>6200</v>
+      </c>
+      <c r="C95">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B96">
+        <v>6300</v>
+      </c>
+      <c r="C96">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B97">
+        <v>6400</v>
+      </c>
+      <c r="C97">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B98">
+        <v>6500</v>
+      </c>
+      <c r="C98">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B99">
+        <v>6600</v>
+      </c>
+      <c r="C99">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B100">
+        <v>6700</v>
+      </c>
+      <c r="C100">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B101">
+        <v>6800</v>
+      </c>
+      <c r="C101">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B102">
+        <v>6900</v>
+      </c>
+      <c r="C102">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B103">
+        <v>7000</v>
+      </c>
+      <c r="C103">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B104">
+        <v>7100</v>
+      </c>
+      <c r="C104">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B105">
+        <v>7200</v>
+      </c>
+      <c r="C105">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B106">
+        <v>7300</v>
+      </c>
+      <c r="C106">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B107">
+        <v>7400</v>
+      </c>
+      <c r="C107">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B108">
+        <v>7500</v>
+      </c>
+      <c r="C108">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B109">
+        <v>7600</v>
+      </c>
+      <c r="C109">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B110">
+        <v>7700</v>
+      </c>
+      <c r="C110">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B111">
+        <v>7800</v>
+      </c>
+      <c r="C111">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B112">
+        <v>7900</v>
+      </c>
+      <c r="C112">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B113">
+        <v>8000</v>
+      </c>
+      <c r="C113">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B114">
+        <v>8100</v>
+      </c>
+      <c r="C114">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B115">
+        <v>8200</v>
+      </c>
+      <c r="C115">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B116">
+        <v>8300</v>
+      </c>
+      <c r="C116">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B117">
+        <v>8400</v>
+      </c>
+      <c r="C117">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B118">
+        <v>8500</v>
+      </c>
+      <c r="C118">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B119">
+        <v>8600</v>
+      </c>
+      <c r="C119">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B120">
+        <v>8700</v>
+      </c>
+      <c r="C120">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B121">
+        <v>8800</v>
+      </c>
+      <c r="C121">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B122">
+        <v>8900</v>
+      </c>
+      <c r="C122">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B123">
+        <v>9000</v>
+      </c>
+      <c r="C123">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B124">
+        <v>9100</v>
+      </c>
+      <c r="C124">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="125" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B125">
+        <v>9200</v>
+      </c>
+      <c r="C125">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B126">
+        <v>9300</v>
+      </c>
+      <c r="C126">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B127">
+        <v>9400</v>
+      </c>
+      <c r="C127">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="128" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B128">
+        <v>9500</v>
+      </c>
+      <c r="C128">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B129">
+        <v>9600</v>
+      </c>
+      <c r="C129">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B130">
+        <v>9700</v>
+      </c>
+      <c r="C130">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="131" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B131">
+        <v>9800</v>
+      </c>
+      <c r="C131">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="132" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B132">
+        <v>9900</v>
+      </c>
+      <c r="C132">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B133">
+        <v>10000</v>
+      </c>
+      <c r="C133">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>